<commit_message>
adding TS parameters to ontology
</commit_message>
<xml_diff>
--- a/data/source/ts_subset_imputed.xlsx
+++ b/data/source/ts_subset_imputed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoliva/GitHub/CTDasRDF/data/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5C526B-0FEC-6740-8118-7BD402E62636}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360E5DF8-E0E2-3B43-9609-BD348E2FC346}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25220" yWindow="-15000" windowWidth="25220" windowHeight="17000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="460" windowWidth="25220" windowHeight="17000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ts_subset.csv" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="166">
   <si>
     <t>studyid</t>
   </si>
@@ -514,6 +514,15 @@
   </si>
   <si>
     <t>study:hasLongTitle</t>
+  </si>
+  <si>
+    <t>2015-03-31</t>
+  </si>
+  <si>
+    <t>2012-07-06</t>
+  </si>
+  <si>
+    <t>2015-03-05</t>
   </si>
 </sst>
 </file>
@@ -562,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -573,6 +582,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -914,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E29" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1978,7 +1990,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1997,8 +2009,8 @@
       <c r="F39" t="s">
         <v>111</v>
       </c>
-      <c r="G39" s="1">
-        <v>40632</v>
+      <c r="G39" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="J39" t="s">
         <v>112</v>
@@ -2091,7 +2103,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2110,8 +2122,8 @@
       <c r="F43" t="s">
         <v>123</v>
       </c>
-      <c r="G43" s="1">
-        <v>39634</v>
+      <c r="G43" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="J43" t="s">
         <v>112</v>
@@ -2120,7 +2132,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2139,8 +2151,8 @@
       <c r="F44" t="s">
         <v>125</v>
       </c>
-      <c r="G44" s="1">
-        <v>40606</v>
+      <c r="G44" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="J44" t="s">
         <v>112</v>

</xml_diff>